<commit_message>
editing excel workbook in python
</commit_message>
<xml_diff>
--- a/pythonprojects/transactions.xlsx
+++ b/pythonprojects/transactions.xlsx
@@ -13,7 +13,7 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -43,6 +43,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -102,8 +103,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -130,58 +135,58 @@
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
         <v>1001</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>5.95</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>5.355</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
         <v>1002</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>6.96</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>6.255</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
         <v>1003</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>7.95</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>7.155</v>
       </c>
     </row>
@@ -190,8 +195,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>